<commit_message>
updated post_process excel file
</commit_message>
<xml_diff>
--- a/PEER_Verification_Test/Fractiles/Post_Process.xlsx
+++ b/PEER_Verification_Test/Fractiles/Post_Process.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmurphy\Desktop\Hazard_Codes\02-Testing\fractiles_testing_Aug2\PEER_Verification_Test\Fractiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="300" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7695" yWindow="300" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Post_Process" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -120,6 +125,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -445,15 +458,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T111"/>
+  <dimension ref="B1:U221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O210" sqref="O210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:20">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -464,7 +477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>1E-3</v>
       </c>
@@ -520,7 +533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:20">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.01</v>
       </c>
@@ -579,7 +592,7 @@
         <v>7.3799999999999996E-6</v>
       </c>
     </row>
-    <row r="4" spans="2:20">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.02</v>
       </c>
@@ -638,7 +651,7 @@
         <v>9.7200000000000001E-6</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.03</v>
       </c>
@@ -697,7 +710,7 @@
         <v>9.7200000000000001E-6</v>
       </c>
     </row>
-    <row r="6" spans="2:20">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.04</v>
       </c>
@@ -756,7 +769,7 @@
         <v>1.4579999999999999E-5</v>
       </c>
     </row>
-    <row r="7" spans="2:20">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.05</v>
       </c>
@@ -815,7 +828,7 @@
         <v>1.4579999999999999E-5</v>
       </c>
     </row>
-    <row r="8" spans="2:20">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.06</v>
       </c>
@@ -874,7 +887,7 @@
         <v>1.4579999999999999E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -933,7 +946,7 @@
         <v>1.519E-5</v>
       </c>
     </row>
-    <row r="10" spans="2:20">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.08</v>
       </c>
@@ -992,7 +1005,7 @@
         <v>1.519E-5</v>
       </c>
     </row>
-    <row r="11" spans="2:20">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.09</v>
       </c>
@@ -1051,7 +1064,7 @@
         <v>1.8859999999999999E-5</v>
       </c>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.1</v>
       </c>
@@ -1110,7 +1123,7 @@
         <v>1.8859999999999999E-5</v>
       </c>
     </row>
-    <row r="13" spans="2:20">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.11</v>
       </c>
@@ -1169,7 +1182,7 @@
         <v>2.207E-5</v>
       </c>
     </row>
-    <row r="14" spans="2:20">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.12</v>
       </c>
@@ -1228,7 +1241,7 @@
         <v>2.2140000000000001E-5</v>
       </c>
     </row>
-    <row r="15" spans="2:20">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0.13</v>
       </c>
@@ -1287,7 +1300,7 @@
         <v>2.2140000000000001E-5</v>
       </c>
     </row>
-    <row r="16" spans="2:20">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.14000000000000001</v>
       </c>
@@ -1346,7 +1359,7 @@
         <v>2.2140000000000001E-5</v>
       </c>
     </row>
-    <row r="17" spans="2:20">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.15</v>
       </c>
@@ -1405,7 +1418,7 @@
         <v>2.2140000000000001E-5</v>
       </c>
     </row>
-    <row r="18" spans="2:20">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0.16</v>
       </c>
@@ -1464,7 +1477,7 @@
         <v>2.2140000000000001E-5</v>
       </c>
     </row>
-    <row r="19" spans="2:20">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.17</v>
       </c>
@@ -1523,7 +1536,7 @@
         <v>2.2379999999999999E-5</v>
       </c>
     </row>
-    <row r="20" spans="2:20">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.18</v>
       </c>
@@ -1582,7 +1595,7 @@
         <v>2.287E-5</v>
       </c>
     </row>
-    <row r="21" spans="2:20">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.19</v>
       </c>
@@ -1641,7 +1654,7 @@
         <v>2.287E-5</v>
       </c>
     </row>
-    <row r="22" spans="2:20">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.2</v>
       </c>
@@ -1682,7 +1695,7 @@
         <v>5.53E-4</v>
       </c>
       <c r="O22" s="1">
-        <v>3.9580000000000003E-4</v>
+        <v>3.9589999999999997E-4</v>
       </c>
       <c r="P22" s="1">
         <v>2.7960000000000002E-4</v>
@@ -1700,7 +1713,7 @@
         <v>2.6319999999999999E-5</v>
       </c>
     </row>
-    <row r="23" spans="2:20">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.21</v>
       </c>
@@ -1759,7 +1772,7 @@
         <v>2.6319999999999999E-5</v>
       </c>
     </row>
-    <row r="24" spans="2:20">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.22</v>
       </c>
@@ -1818,7 +1831,7 @@
         <v>2.6740000000000001E-5</v>
       </c>
     </row>
-    <row r="25" spans="2:20">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0.23</v>
       </c>
@@ -1877,7 +1890,7 @@
         <v>2.8819999999999999E-5</v>
       </c>
     </row>
-    <row r="26" spans="2:20">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.24</v>
       </c>
@@ -1936,7 +1949,7 @@
         <v>2.8819999999999999E-5</v>
       </c>
     </row>
-    <row r="27" spans="2:20">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.25</v>
       </c>
@@ -1995,7 +2008,7 @@
         <v>2.9159999999999999E-5</v>
       </c>
     </row>
-    <row r="28" spans="2:20">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.26</v>
       </c>
@@ -2054,7 +2067,7 @@
         <v>2.9159999999999999E-5</v>
       </c>
     </row>
-    <row r="29" spans="2:20">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.27</v>
       </c>
@@ -2113,7 +2126,7 @@
         <v>2.9159999999999999E-5</v>
       </c>
     </row>
-    <row r="30" spans="2:20">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.28000000000000003</v>
       </c>
@@ -2172,7 +2185,7 @@
         <v>2.9159999999999999E-5</v>
       </c>
     </row>
-    <row r="31" spans="2:20">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.28999999999999998</v>
       </c>
@@ -2231,7 +2244,7 @@
         <v>2.9159999999999999E-5</v>
       </c>
     </row>
-    <row r="32" spans="2:20">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.3</v>
       </c>
@@ -2290,7 +2303,7 @@
         <v>2.9689999999999999E-5</v>
       </c>
     </row>
-    <row r="33" spans="2:20">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.31</v>
       </c>
@@ -2349,7 +2362,7 @@
         <v>4.3739999999999998E-5</v>
       </c>
     </row>
-    <row r="34" spans="2:20">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0.32</v>
       </c>
@@ -2408,7 +2421,7 @@
         <v>4.3739999999999998E-5</v>
       </c>
     </row>
-    <row r="35" spans="2:20">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.33</v>
       </c>
@@ -2467,7 +2480,7 @@
         <v>4.3739999999999998E-5</v>
       </c>
     </row>
-    <row r="36" spans="2:20">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0.34</v>
       </c>
@@ -2526,7 +2539,7 @@
         <v>4.3739999999999998E-5</v>
       </c>
     </row>
-    <row r="37" spans="2:20">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0.35</v>
       </c>
@@ -2585,7 +2598,7 @@
         <v>4.3739999999999998E-5</v>
       </c>
     </row>
-    <row r="38" spans="2:20">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0.36</v>
       </c>
@@ -2644,7 +2657,7 @@
         <v>4.3739999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="2:20">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.37</v>
       </c>
@@ -2703,7 +2716,7 @@
         <v>4.3739999999999998E-5</v>
       </c>
     </row>
-    <row r="40" spans="2:20">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0.38</v>
       </c>
@@ -2762,7 +2775,7 @@
         <v>4.5559999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="2:20">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.39</v>
       </c>
@@ -2821,7 +2834,7 @@
         <v>4.5559999999999997E-5</v>
       </c>
     </row>
-    <row r="42" spans="2:20">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>0.4</v>
       </c>
@@ -2880,7 +2893,7 @@
         <v>4.5559999999999997E-5</v>
       </c>
     </row>
-    <row r="43" spans="2:20">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>0.41</v>
       </c>
@@ -2939,7 +2952,7 @@
         <v>4.5559999999999997E-5</v>
       </c>
     </row>
-    <row r="44" spans="2:20">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>0.42</v>
       </c>
@@ -2998,7 +3011,7 @@
         <v>4.5559999999999997E-5</v>
       </c>
     </row>
-    <row r="45" spans="2:20">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>0.43</v>
       </c>
@@ -3057,7 +3070,7 @@
         <v>4.5559999999999997E-5</v>
       </c>
     </row>
-    <row r="46" spans="2:20">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>0.44</v>
       </c>
@@ -3116,7 +3129,7 @@
         <v>4.5559999999999997E-5</v>
       </c>
     </row>
-    <row r="47" spans="2:20">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>0.45</v>
       </c>
@@ -3175,7 +3188,7 @@
         <v>4.5559999999999997E-5</v>
       </c>
     </row>
-    <row r="48" spans="2:20">
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>0.46</v>
       </c>
@@ -3234,7 +3247,7 @@
         <v>5.6570000000000002E-5</v>
       </c>
     </row>
-    <row r="49" spans="2:20">
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>0.47</v>
       </c>
@@ -3293,7 +3306,7 @@
         <v>5.6570000000000002E-5</v>
       </c>
     </row>
-    <row r="50" spans="2:20">
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>0.48</v>
       </c>
@@ -3352,7 +3365,7 @@
         <v>5.6570000000000002E-5</v>
       </c>
     </row>
-    <row r="51" spans="2:20">
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>0.49</v>
       </c>
@@ -3411,7 +3424,7 @@
         <v>5.6570000000000002E-5</v>
       </c>
     </row>
-    <row r="52" spans="2:20">
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>0.5</v>
       </c>
@@ -3470,7 +3483,7 @@
         <v>5.6570000000000002E-5</v>
       </c>
     </row>
-    <row r="53" spans="2:20">
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>0.51</v>
       </c>
@@ -3529,7 +3542,7 @@
         <v>6.6199999999999996E-5</v>
       </c>
     </row>
-    <row r="54" spans="2:20">
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>0.52</v>
       </c>
@@ -3588,7 +3601,7 @@
         <v>6.6199999999999996E-5</v>
       </c>
     </row>
-    <row r="55" spans="2:20">
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>0.53</v>
       </c>
@@ -3647,7 +3660,7 @@
         <v>6.6199999999999996E-5</v>
       </c>
     </row>
-    <row r="56" spans="2:20">
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>0.54</v>
       </c>
@@ -3706,7 +3719,7 @@
         <v>6.6199999999999996E-5</v>
       </c>
     </row>
-    <row r="57" spans="2:20">
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>0.55000000000000004</v>
       </c>
@@ -3765,7 +3778,7 @@
         <v>6.7150000000000006E-5</v>
       </c>
     </row>
-    <row r="58" spans="2:20">
+    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>0.56000000000000005</v>
       </c>
@@ -3824,7 +3837,7 @@
         <v>6.7150000000000006E-5</v>
       </c>
     </row>
-    <row r="59" spans="2:20">
+    <row r="59" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>0.56999999999999995</v>
       </c>
@@ -3883,7 +3896,7 @@
         <v>6.7150000000000006E-5</v>
       </c>
     </row>
-    <row r="60" spans="2:20">
+    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>0.57999999999999996</v>
       </c>
@@ -3942,7 +3955,7 @@
         <v>6.8609999999999995E-5</v>
       </c>
     </row>
-    <row r="61" spans="2:20">
+    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>0.59</v>
       </c>
@@ -4001,7 +4014,7 @@
         <v>6.8609999999999995E-5</v>
       </c>
     </row>
-    <row r="62" spans="2:20">
+    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>0.6</v>
       </c>
@@ -4060,7 +4073,7 @@
         <v>6.8609999999999995E-5</v>
       </c>
     </row>
-    <row r="63" spans="2:20">
+    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>0.61</v>
       </c>
@@ -4119,7 +4132,7 @@
         <v>6.8609999999999995E-5</v>
       </c>
     </row>
-    <row r="64" spans="2:20">
+    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>0.62</v>
       </c>
@@ -4178,7 +4191,7 @@
         <v>6.8609999999999995E-5</v>
       </c>
     </row>
-    <row r="65" spans="2:20">
+    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>0.63</v>
       </c>
@@ -4237,7 +4250,7 @@
         <v>6.8609999999999995E-5</v>
       </c>
     </row>
-    <row r="66" spans="2:20">
+    <row r="66" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>0.64</v>
       </c>
@@ -4296,7 +4309,7 @@
         <v>7.3800000000000005E-5</v>
       </c>
     </row>
-    <row r="67" spans="2:20">
+    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>0.65</v>
       </c>
@@ -4355,7 +4368,7 @@
         <v>7.3800000000000005E-5</v>
       </c>
     </row>
-    <row r="68" spans="2:20">
+    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>0.66</v>
       </c>
@@ -4414,7 +4427,7 @@
         <v>7.8949999999999995E-5</v>
       </c>
     </row>
-    <row r="69" spans="2:20">
+    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>0.67</v>
       </c>
@@ -4473,7 +4486,7 @@
         <v>7.8949999999999995E-5</v>
       </c>
     </row>
-    <row r="70" spans="2:20">
+    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>0.68</v>
       </c>
@@ -4532,7 +4545,7 @@
         <v>7.8949999999999995E-5</v>
       </c>
     </row>
-    <row r="71" spans="2:20">
+    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>0.69</v>
       </c>
@@ -4591,7 +4604,7 @@
         <v>7.8949999999999995E-5</v>
       </c>
     </row>
-    <row r="72" spans="2:20">
+    <row r="72" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>0.7</v>
       </c>
@@ -4650,7 +4663,7 @@
         <v>8.0220000000000001E-5</v>
       </c>
     </row>
-    <row r="73" spans="2:20">
+    <row r="73" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>0.71</v>
       </c>
@@ -4709,7 +4722,7 @@
         <v>8.0220000000000001E-5</v>
       </c>
     </row>
-    <row r="74" spans="2:20">
+    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>0.72</v>
       </c>
@@ -4768,7 +4781,7 @@
         <v>8.0220000000000001E-5</v>
       </c>
     </row>
-    <row r="75" spans="2:20">
+    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>0.73</v>
       </c>
@@ -4827,7 +4840,7 @@
         <v>8.0220000000000001E-5</v>
       </c>
     </row>
-    <row r="76" spans="2:20">
+    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>0.74</v>
       </c>
@@ -4886,7 +4899,7 @@
         <v>8.0220000000000001E-5</v>
       </c>
     </row>
-    <row r="77" spans="2:20">
+    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>0.75</v>
       </c>
@@ -4945,7 +4958,7 @@
         <v>8.6450000000000001E-5</v>
       </c>
     </row>
-    <row r="78" spans="2:20">
+    <row r="78" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>0.76</v>
       </c>
@@ -5004,7 +5017,7 @@
         <v>8.6450000000000001E-5</v>
       </c>
     </row>
-    <row r="79" spans="2:20">
+    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>0.77</v>
       </c>
@@ -5063,7 +5076,7 @@
         <v>8.6450000000000001E-5</v>
       </c>
     </row>
-    <row r="80" spans="2:20">
+    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>0.78</v>
       </c>
@@ -5122,7 +5135,7 @@
         <v>8.6450000000000001E-5</v>
       </c>
     </row>
-    <row r="81" spans="2:20">
+    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>0.79</v>
       </c>
@@ -5181,7 +5194,7 @@
         <v>8.9069999999999999E-5</v>
       </c>
     </row>
-    <row r="82" spans="2:20">
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>0.8</v>
       </c>
@@ -5240,7 +5253,7 @@
         <v>8.9069999999999999E-5</v>
       </c>
     </row>
-    <row r="83" spans="2:20">
+    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>0.81</v>
       </c>
@@ -5299,7 +5312,7 @@
         <v>8.9069999999999999E-5</v>
       </c>
     </row>
-    <row r="84" spans="2:20">
+    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>0.82</v>
       </c>
@@ -5358,7 +5371,7 @@
         <v>9.7200000000000004E-5</v>
       </c>
     </row>
-    <row r="85" spans="2:20">
+    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>0.83</v>
       </c>
@@ -5417,7 +5430,7 @@
         <v>9.7200000000000004E-5</v>
       </c>
     </row>
-    <row r="86" spans="2:20">
+    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>0.84</v>
       </c>
@@ -5476,7 +5489,7 @@
         <v>1.4579999999999999E-4</v>
       </c>
     </row>
-    <row r="87" spans="2:20">
+    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>0.85</v>
       </c>
@@ -5535,7 +5548,7 @@
         <v>1.4579999999999999E-4</v>
       </c>
     </row>
-    <row r="88" spans="2:20">
+    <row r="88" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>0.86</v>
       </c>
@@ -5594,7 +5607,7 @@
         <v>1.5190000000000001E-4</v>
       </c>
     </row>
-    <row r="89" spans="2:20">
+    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>0.87</v>
       </c>
@@ -5653,7 +5666,7 @@
         <v>1.5190000000000001E-4</v>
       </c>
     </row>
-    <row r="90" spans="2:20">
+    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>0.88</v>
       </c>
@@ -5712,7 +5725,7 @@
         <v>1.5190000000000001E-4</v>
       </c>
     </row>
-    <row r="91" spans="2:20">
+    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>0.89</v>
       </c>
@@ -5771,7 +5784,7 @@
         <v>1.886E-4</v>
       </c>
     </row>
-    <row r="92" spans="2:20">
+    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>0.9</v>
       </c>
@@ -5830,7 +5843,7 @@
         <v>1.886E-4</v>
       </c>
     </row>
-    <row r="93" spans="2:20">
+    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>0.91</v>
       </c>
@@ -5889,7 +5902,7 @@
         <v>2.207E-4</v>
       </c>
     </row>
-    <row r="94" spans="2:20">
+    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>0.92</v>
       </c>
@@ -5948,7 +5961,7 @@
         <v>2.2379999999999999E-4</v>
       </c>
     </row>
-    <row r="95" spans="2:20">
+    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>0.93</v>
       </c>
@@ -6007,7 +6020,7 @@
         <v>2.287E-4</v>
       </c>
     </row>
-    <row r="96" spans="2:20">
+    <row r="96" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>0.94</v>
       </c>
@@ -6066,7 +6079,7 @@
         <v>2.287E-4</v>
       </c>
     </row>
-    <row r="97" spans="2:20">
+    <row r="97" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>0.95</v>
       </c>
@@ -6107,7 +6120,7 @@
         <v>5.5300000000000002E-3</v>
       </c>
       <c r="O97" s="1">
-        <v>3.9579999999999997E-3</v>
+        <v>3.9589999999999998E-3</v>
       </c>
       <c r="P97" s="1">
         <v>2.7959999999999999E-3</v>
@@ -6125,7 +6138,7 @@
         <v>2.632E-4</v>
       </c>
     </row>
-    <row r="98" spans="2:20">
+    <row r="98" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>0.96</v>
       </c>
@@ -6184,7 +6197,7 @@
         <v>2.632E-4</v>
       </c>
     </row>
-    <row r="99" spans="2:20">
+    <row r="99" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>0.97</v>
       </c>
@@ -6243,7 +6256,7 @@
         <v>2.6739999999999999E-4</v>
       </c>
     </row>
-    <row r="100" spans="2:20">
+    <row r="100" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>0.98</v>
       </c>
@@ -6302,7 +6315,7 @@
         <v>2.8820000000000001E-4</v>
       </c>
     </row>
-    <row r="101" spans="2:20">
+    <row r="101" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>0.99</v>
       </c>
@@ -6361,14 +6374,14 @@
         <v>2.9690000000000001E-4</v>
       </c>
     </row>
-    <row r="103" spans="2:20">
+    <row r="103" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
     </row>
-    <row r="105" spans="2:20">
+    <row r="105" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B105">
         <f>B12</f>
         <v>0.1</v>
@@ -6446,7 +6459,7 @@
         <v>1.8859822151329197E-5</v>
       </c>
     </row>
-    <row r="106" spans="2:20">
+    <row r="106" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B106">
         <f>B52</f>
         <v>0.5</v>
@@ -6524,7 +6537,7 @@
         <v>5.6568399947720671E-5</v>
       </c>
     </row>
-    <row r="107" spans="2:20">
+    <row r="107" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B107">
         <f>B92</f>
         <v>0.9</v>
@@ -6602,12 +6615,11 @@
         <v>1.885822161380446E-4</v>
       </c>
     </row>
-    <row r="109" spans="2:20">
+    <row r="109" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
     </row>
-    <row r="111" spans="2:20">
-      <c r="C111" s="1"/>
+    <row r="111" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -6625,6 +6637,2017 @@
       <c r="R111" s="1"/>
       <c r="S111" s="1"/>
       <c r="T111" s="1"/>
+      <c r="U111" s="1"/>
+    </row>
+    <row r="112" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1"/>
+      <c r="P112" s="1"/>
+      <c r="Q112" s="1"/>
+      <c r="R112" s="1"/>
+      <c r="S112" s="1"/>
+      <c r="T112" s="1"/>
+    </row>
+    <row r="113" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+      <c r="Q113" s="1"/>
+      <c r="R113" s="1"/>
+      <c r="S113" s="1"/>
+      <c r="T113" s="1"/>
+    </row>
+    <row r="114" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1"/>
+      <c r="P114" s="1"/>
+      <c r="Q114" s="1"/>
+      <c r="R114" s="1"/>
+      <c r="S114" s="1"/>
+      <c r="T114" s="1"/>
+    </row>
+    <row r="115" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+      <c r="N115" s="1"/>
+      <c r="O115" s="1"/>
+      <c r="P115" s="1"/>
+      <c r="Q115" s="1"/>
+      <c r="R115" s="1"/>
+      <c r="S115" s="1"/>
+      <c r="T115" s="1"/>
+    </row>
+    <row r="116" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1"/>
+      <c r="N116" s="1"/>
+      <c r="O116" s="1"/>
+      <c r="P116" s="1"/>
+      <c r="Q116" s="1"/>
+      <c r="R116" s="1"/>
+      <c r="S116" s="1"/>
+      <c r="T116" s="1"/>
+    </row>
+    <row r="117" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+      <c r="N117" s="1"/>
+      <c r="O117" s="1"/>
+      <c r="P117" s="1"/>
+      <c r="Q117" s="1"/>
+      <c r="R117" s="1"/>
+      <c r="S117" s="1"/>
+      <c r="T117" s="1"/>
+    </row>
+    <row r="118" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+      <c r="N118" s="1"/>
+      <c r="O118" s="1"/>
+      <c r="P118" s="1"/>
+      <c r="Q118" s="1"/>
+      <c r="R118" s="1"/>
+      <c r="S118" s="1"/>
+      <c r="T118" s="1"/>
+    </row>
+    <row r="119" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+      <c r="L119" s="1"/>
+      <c r="M119" s="1"/>
+      <c r="N119" s="1"/>
+      <c r="O119" s="1"/>
+      <c r="P119" s="1"/>
+      <c r="Q119" s="1"/>
+      <c r="R119" s="1"/>
+      <c r="S119" s="1"/>
+      <c r="T119" s="1"/>
+    </row>
+    <row r="120" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+      <c r="L120" s="1"/>
+      <c r="M120" s="1"/>
+      <c r="N120" s="1"/>
+      <c r="O120" s="1"/>
+      <c r="P120" s="1"/>
+      <c r="Q120" s="1"/>
+      <c r="R120" s="1"/>
+      <c r="S120" s="1"/>
+      <c r="T120" s="1"/>
+    </row>
+    <row r="121" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+      <c r="L121" s="1"/>
+      <c r="M121" s="1"/>
+      <c r="N121" s="1"/>
+      <c r="O121" s="1"/>
+      <c r="P121" s="1"/>
+      <c r="Q121" s="1"/>
+      <c r="R121" s="1"/>
+      <c r="S121" s="1"/>
+      <c r="T121" s="1"/>
+    </row>
+    <row r="122" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+      <c r="O122" s="1"/>
+      <c r="P122" s="1"/>
+      <c r="Q122" s="1"/>
+      <c r="R122" s="1"/>
+      <c r="S122" s="1"/>
+      <c r="T122" s="1"/>
+    </row>
+    <row r="123" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+      <c r="L123" s="1"/>
+      <c r="M123" s="1"/>
+      <c r="N123" s="1"/>
+      <c r="O123" s="1"/>
+      <c r="P123" s="1"/>
+      <c r="Q123" s="1"/>
+      <c r="R123" s="1"/>
+      <c r="S123" s="1"/>
+      <c r="T123" s="1"/>
+    </row>
+    <row r="124" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+      <c r="L124" s="1"/>
+      <c r="M124" s="1"/>
+      <c r="N124" s="1"/>
+      <c r="O124" s="1"/>
+      <c r="P124" s="1"/>
+      <c r="Q124" s="1"/>
+      <c r="R124" s="1"/>
+      <c r="S124" s="1"/>
+      <c r="T124" s="1"/>
+    </row>
+    <row r="125" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+      <c r="J125" s="1"/>
+      <c r="K125" s="1"/>
+      <c r="L125" s="1"/>
+      <c r="M125" s="1"/>
+      <c r="N125" s="1"/>
+      <c r="O125" s="1"/>
+      <c r="P125" s="1"/>
+      <c r="Q125" s="1"/>
+      <c r="R125" s="1"/>
+      <c r="S125" s="1"/>
+      <c r="T125" s="1"/>
+    </row>
+    <row r="126" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
+      <c r="O126" s="1"/>
+      <c r="P126" s="1"/>
+      <c r="Q126" s="1"/>
+      <c r="R126" s="1"/>
+      <c r="S126" s="1"/>
+      <c r="T126" s="1"/>
+    </row>
+    <row r="127" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+      <c r="K127" s="1"/>
+      <c r="L127" s="1"/>
+      <c r="M127" s="1"/>
+      <c r="N127" s="1"/>
+      <c r="O127" s="1"/>
+      <c r="P127" s="1"/>
+      <c r="Q127" s="1"/>
+      <c r="R127" s="1"/>
+      <c r="S127" s="1"/>
+      <c r="T127" s="1"/>
+    </row>
+    <row r="128" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
+      <c r="K128" s="1"/>
+      <c r="L128" s="1"/>
+      <c r="M128" s="1"/>
+      <c r="N128" s="1"/>
+      <c r="O128" s="1"/>
+      <c r="P128" s="1"/>
+      <c r="Q128" s="1"/>
+      <c r="R128" s="1"/>
+      <c r="S128" s="1"/>
+      <c r="T128" s="1"/>
+    </row>
+    <row r="129" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="1"/>
+      <c r="J129" s="1"/>
+      <c r="K129" s="1"/>
+      <c r="L129" s="1"/>
+      <c r="M129" s="1"/>
+      <c r="N129" s="1"/>
+      <c r="O129" s="1"/>
+      <c r="P129" s="1"/>
+      <c r="Q129" s="1"/>
+      <c r="R129" s="1"/>
+      <c r="S129" s="1"/>
+      <c r="T129" s="1"/>
+    </row>
+    <row r="130" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+      <c r="L130" s="1"/>
+      <c r="M130" s="1"/>
+      <c r="N130" s="1"/>
+      <c r="O130" s="1"/>
+      <c r="P130" s="1"/>
+      <c r="Q130" s="1"/>
+      <c r="R130" s="1"/>
+      <c r="S130" s="1"/>
+      <c r="T130" s="1"/>
+    </row>
+    <row r="131" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+      <c r="L131" s="1"/>
+      <c r="M131" s="1"/>
+      <c r="N131" s="1"/>
+      <c r="O131" s="1"/>
+      <c r="P131" s="1"/>
+      <c r="Q131" s="1"/>
+      <c r="R131" s="1"/>
+      <c r="S131" s="1"/>
+      <c r="T131" s="1"/>
+    </row>
+    <row r="132" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
+      <c r="O132" s="1"/>
+      <c r="P132" s="1"/>
+      <c r="Q132" s="1"/>
+      <c r="R132" s="1"/>
+      <c r="S132" s="1"/>
+      <c r="T132" s="1"/>
+    </row>
+    <row r="133" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="N133" s="1"/>
+      <c r="O133" s="1"/>
+      <c r="P133" s="1"/>
+      <c r="Q133" s="1"/>
+      <c r="R133" s="1"/>
+      <c r="S133" s="1"/>
+      <c r="T133" s="1"/>
+    </row>
+    <row r="134" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
+      <c r="O134" s="1"/>
+      <c r="P134" s="1"/>
+      <c r="Q134" s="1"/>
+      <c r="R134" s="1"/>
+      <c r="S134" s="1"/>
+      <c r="T134" s="1"/>
+    </row>
+    <row r="135" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+      <c r="O135" s="1"/>
+      <c r="P135" s="1"/>
+      <c r="Q135" s="1"/>
+      <c r="R135" s="1"/>
+      <c r="S135" s="1"/>
+      <c r="T135" s="1"/>
+    </row>
+    <row r="136" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="M136" s="1"/>
+      <c r="N136" s="1"/>
+      <c r="O136" s="1"/>
+      <c r="P136" s="1"/>
+      <c r="Q136" s="1"/>
+      <c r="R136" s="1"/>
+      <c r="S136" s="1"/>
+      <c r="T136" s="1"/>
+    </row>
+    <row r="137" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+      <c r="L137" s="1"/>
+      <c r="M137" s="1"/>
+      <c r="N137" s="1"/>
+      <c r="O137" s="1"/>
+      <c r="P137" s="1"/>
+      <c r="Q137" s="1"/>
+      <c r="R137" s="1"/>
+      <c r="S137" s="1"/>
+      <c r="T137" s="1"/>
+    </row>
+    <row r="138" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="M138" s="1"/>
+      <c r="N138" s="1"/>
+      <c r="O138" s="1"/>
+      <c r="P138" s="1"/>
+      <c r="Q138" s="1"/>
+      <c r="R138" s="1"/>
+      <c r="S138" s="1"/>
+      <c r="T138" s="1"/>
+    </row>
+    <row r="139" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="M139" s="1"/>
+      <c r="N139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
+      <c r="Q139" s="1"/>
+      <c r="R139" s="1"/>
+      <c r="S139" s="1"/>
+      <c r="T139" s="1"/>
+    </row>
+    <row r="140" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="M140" s="1"/>
+      <c r="N140" s="1"/>
+      <c r="O140" s="1"/>
+      <c r="P140" s="1"/>
+      <c r="Q140" s="1"/>
+      <c r="R140" s="1"/>
+      <c r="S140" s="1"/>
+      <c r="T140" s="1"/>
+    </row>
+    <row r="141" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="M141" s="1"/>
+      <c r="N141" s="1"/>
+      <c r="O141" s="1"/>
+      <c r="P141" s="1"/>
+      <c r="Q141" s="1"/>
+      <c r="R141" s="1"/>
+      <c r="S141" s="1"/>
+      <c r="T141" s="1"/>
+    </row>
+    <row r="142" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="M142" s="1"/>
+      <c r="N142" s="1"/>
+      <c r="O142" s="1"/>
+      <c r="P142" s="1"/>
+      <c r="Q142" s="1"/>
+      <c r="R142" s="1"/>
+      <c r="S142" s="1"/>
+      <c r="T142" s="1"/>
+    </row>
+    <row r="143" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1"/>
+      <c r="L143" s="1"/>
+      <c r="M143" s="1"/>
+      <c r="N143" s="1"/>
+      <c r="O143" s="1"/>
+      <c r="P143" s="1"/>
+      <c r="Q143" s="1"/>
+      <c r="R143" s="1"/>
+      <c r="S143" s="1"/>
+      <c r="T143" s="1"/>
+    </row>
+    <row r="144" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+      <c r="I144" s="1"/>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="M144" s="1"/>
+      <c r="N144" s="1"/>
+      <c r="O144" s="1"/>
+      <c r="P144" s="1"/>
+      <c r="Q144" s="1"/>
+      <c r="R144" s="1"/>
+      <c r="S144" s="1"/>
+      <c r="T144" s="1"/>
+    </row>
+    <row r="145" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C145" s="1"/>
+      <c r="D145" s="1"/>
+      <c r="E145" s="1"/>
+      <c r="F145" s="1"/>
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
+      <c r="I145" s="1"/>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1"/>
+      <c r="L145" s="1"/>
+      <c r="M145" s="1"/>
+      <c r="N145" s="1"/>
+      <c r="O145" s="1"/>
+      <c r="P145" s="1"/>
+      <c r="Q145" s="1"/>
+      <c r="R145" s="1"/>
+      <c r="S145" s="1"/>
+      <c r="T145" s="1"/>
+    </row>
+    <row r="146" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+      <c r="L146" s="1"/>
+      <c r="M146" s="1"/>
+      <c r="N146" s="1"/>
+      <c r="O146" s="1"/>
+      <c r="P146" s="1"/>
+      <c r="Q146" s="1"/>
+      <c r="R146" s="1"/>
+      <c r="S146" s="1"/>
+      <c r="T146" s="1"/>
+    </row>
+    <row r="147" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="1"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
+      <c r="J147" s="1"/>
+      <c r="K147" s="1"/>
+      <c r="L147" s="1"/>
+      <c r="M147" s="1"/>
+      <c r="N147" s="1"/>
+      <c r="O147" s="1"/>
+      <c r="P147" s="1"/>
+      <c r="Q147" s="1"/>
+      <c r="R147" s="1"/>
+      <c r="S147" s="1"/>
+      <c r="T147" s="1"/>
+    </row>
+    <row r="148" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+      <c r="I148" s="1"/>
+      <c r="J148" s="1"/>
+      <c r="K148" s="1"/>
+      <c r="L148" s="1"/>
+      <c r="M148" s="1"/>
+      <c r="N148" s="1"/>
+      <c r="O148" s="1"/>
+      <c r="P148" s="1"/>
+      <c r="Q148" s="1"/>
+      <c r="R148" s="1"/>
+      <c r="S148" s="1"/>
+      <c r="T148" s="1"/>
+    </row>
+    <row r="149" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+      <c r="I149" s="1"/>
+      <c r="J149" s="1"/>
+      <c r="K149" s="1"/>
+      <c r="L149" s="1"/>
+      <c r="M149" s="1"/>
+      <c r="N149" s="1"/>
+      <c r="O149" s="1"/>
+      <c r="P149" s="1"/>
+      <c r="Q149" s="1"/>
+      <c r="R149" s="1"/>
+      <c r="S149" s="1"/>
+      <c r="T149" s="1"/>
+    </row>
+    <row r="150" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="M150" s="1"/>
+      <c r="N150" s="1"/>
+      <c r="O150" s="1"/>
+      <c r="P150" s="1"/>
+      <c r="Q150" s="1"/>
+      <c r="R150" s="1"/>
+      <c r="S150" s="1"/>
+      <c r="T150" s="1"/>
+    </row>
+    <row r="151" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+      <c r="T151" s="1"/>
+    </row>
+    <row r="152" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+      <c r="I152" s="1"/>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+      <c r="L152" s="1"/>
+      <c r="M152" s="1"/>
+      <c r="N152" s="1"/>
+      <c r="O152" s="1"/>
+      <c r="P152" s="1"/>
+      <c r="Q152" s="1"/>
+      <c r="R152" s="1"/>
+      <c r="S152" s="1"/>
+      <c r="T152" s="1"/>
+    </row>
+    <row r="153" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+      <c r="I153" s="1"/>
+      <c r="J153" s="1"/>
+      <c r="K153" s="1"/>
+      <c r="L153" s="1"/>
+      <c r="M153" s="1"/>
+      <c r="N153" s="1"/>
+      <c r="O153" s="1"/>
+      <c r="P153" s="1"/>
+      <c r="Q153" s="1"/>
+      <c r="R153" s="1"/>
+      <c r="S153" s="1"/>
+      <c r="T153" s="1"/>
+    </row>
+    <row r="154" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
+      <c r="I154" s="1"/>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="M154" s="1"/>
+      <c r="N154" s="1"/>
+      <c r="O154" s="1"/>
+      <c r="P154" s="1"/>
+      <c r="Q154" s="1"/>
+      <c r="R154" s="1"/>
+      <c r="S154" s="1"/>
+      <c r="T154" s="1"/>
+    </row>
+    <row r="155" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+      <c r="L155" s="1"/>
+      <c r="M155" s="1"/>
+      <c r="N155" s="1"/>
+      <c r="O155" s="1"/>
+      <c r="P155" s="1"/>
+      <c r="Q155" s="1"/>
+      <c r="R155" s="1"/>
+      <c r="S155" s="1"/>
+      <c r="T155" s="1"/>
+    </row>
+    <row r="156" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+      <c r="N156" s="1"/>
+      <c r="O156" s="1"/>
+      <c r="P156" s="1"/>
+      <c r="Q156" s="1"/>
+      <c r="R156" s="1"/>
+      <c r="S156" s="1"/>
+      <c r="T156" s="1"/>
+    </row>
+    <row r="157" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+      <c r="L157" s="1"/>
+      <c r="M157" s="1"/>
+      <c r="N157" s="1"/>
+      <c r="O157" s="1"/>
+      <c r="P157" s="1"/>
+      <c r="Q157" s="1"/>
+      <c r="R157" s="1"/>
+      <c r="S157" s="1"/>
+      <c r="T157" s="1"/>
+    </row>
+    <row r="158" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
+      <c r="L158" s="1"/>
+      <c r="M158" s="1"/>
+      <c r="N158" s="1"/>
+      <c r="O158" s="1"/>
+      <c r="P158" s="1"/>
+      <c r="Q158" s="1"/>
+      <c r="R158" s="1"/>
+      <c r="S158" s="1"/>
+      <c r="T158" s="1"/>
+    </row>
+    <row r="159" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+      <c r="L159" s="1"/>
+      <c r="M159" s="1"/>
+      <c r="N159" s="1"/>
+      <c r="O159" s="1"/>
+      <c r="P159" s="1"/>
+      <c r="Q159" s="1"/>
+      <c r="R159" s="1"/>
+      <c r="S159" s="1"/>
+      <c r="T159" s="1"/>
+    </row>
+    <row r="160" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
+      <c r="O160" s="1"/>
+      <c r="P160" s="1"/>
+      <c r="Q160" s="1"/>
+      <c r="R160" s="1"/>
+      <c r="S160" s="1"/>
+      <c r="T160" s="1"/>
+    </row>
+    <row r="161" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+      <c r="L161" s="1"/>
+      <c r="M161" s="1"/>
+      <c r="N161" s="1"/>
+      <c r="O161" s="1"/>
+      <c r="P161" s="1"/>
+      <c r="Q161" s="1"/>
+      <c r="R161" s="1"/>
+      <c r="S161" s="1"/>
+      <c r="T161" s="1"/>
+    </row>
+    <row r="162" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1"/>
+      <c r="I162" s="1"/>
+      <c r="J162" s="1"/>
+      <c r="K162" s="1"/>
+      <c r="L162" s="1"/>
+      <c r="M162" s="1"/>
+      <c r="N162" s="1"/>
+      <c r="O162" s="1"/>
+      <c r="P162" s="1"/>
+      <c r="Q162" s="1"/>
+      <c r="R162" s="1"/>
+      <c r="S162" s="1"/>
+      <c r="T162" s="1"/>
+    </row>
+    <row r="163" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
+      <c r="H163" s="1"/>
+      <c r="I163" s="1"/>
+      <c r="J163" s="1"/>
+      <c r="K163" s="1"/>
+      <c r="L163" s="1"/>
+      <c r="M163" s="1"/>
+      <c r="N163" s="1"/>
+      <c r="O163" s="1"/>
+      <c r="P163" s="1"/>
+      <c r="Q163" s="1"/>
+      <c r="R163" s="1"/>
+      <c r="S163" s="1"/>
+      <c r="T163" s="1"/>
+    </row>
+    <row r="164" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="1"/>
+      <c r="H164" s="1"/>
+      <c r="I164" s="1"/>
+      <c r="J164" s="1"/>
+      <c r="K164" s="1"/>
+      <c r="L164" s="1"/>
+      <c r="M164" s="1"/>
+      <c r="N164" s="1"/>
+      <c r="O164" s="1"/>
+      <c r="P164" s="1"/>
+      <c r="Q164" s="1"/>
+      <c r="R164" s="1"/>
+      <c r="S164" s="1"/>
+      <c r="T164" s="1"/>
+    </row>
+    <row r="165" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="1"/>
+      <c r="H165" s="1"/>
+      <c r="I165" s="1"/>
+      <c r="J165" s="1"/>
+      <c r="K165" s="1"/>
+      <c r="L165" s="1"/>
+      <c r="M165" s="1"/>
+      <c r="N165" s="1"/>
+      <c r="O165" s="1"/>
+      <c r="P165" s="1"/>
+      <c r="Q165" s="1"/>
+      <c r="R165" s="1"/>
+      <c r="S165" s="1"/>
+      <c r="T165" s="1"/>
+    </row>
+    <row r="166" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="1"/>
+      <c r="H166" s="1"/>
+      <c r="I166" s="1"/>
+      <c r="J166" s="1"/>
+      <c r="K166" s="1"/>
+      <c r="L166" s="1"/>
+      <c r="M166" s="1"/>
+      <c r="N166" s="1"/>
+      <c r="O166" s="1"/>
+      <c r="P166" s="1"/>
+      <c r="Q166" s="1"/>
+      <c r="R166" s="1"/>
+      <c r="S166" s="1"/>
+      <c r="T166" s="1"/>
+    </row>
+    <row r="167" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="1"/>
+      <c r="H167" s="1"/>
+      <c r="I167" s="1"/>
+      <c r="J167" s="1"/>
+      <c r="K167" s="1"/>
+      <c r="L167" s="1"/>
+      <c r="M167" s="1"/>
+      <c r="N167" s="1"/>
+      <c r="O167" s="1"/>
+      <c r="P167" s="1"/>
+      <c r="Q167" s="1"/>
+      <c r="R167" s="1"/>
+      <c r="S167" s="1"/>
+      <c r="T167" s="1"/>
+    </row>
+    <row r="168" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1"/>
+      <c r="I168" s="1"/>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+      <c r="L168" s="1"/>
+      <c r="M168" s="1"/>
+      <c r="N168" s="1"/>
+      <c r="O168" s="1"/>
+      <c r="P168" s="1"/>
+      <c r="Q168" s="1"/>
+      <c r="R168" s="1"/>
+      <c r="S168" s="1"/>
+      <c r="T168" s="1"/>
+    </row>
+    <row r="169" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1"/>
+      <c r="I169" s="1"/>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
+      <c r="L169" s="1"/>
+      <c r="M169" s="1"/>
+      <c r="N169" s="1"/>
+      <c r="O169" s="1"/>
+      <c r="P169" s="1"/>
+      <c r="Q169" s="1"/>
+      <c r="R169" s="1"/>
+      <c r="S169" s="1"/>
+      <c r="T169" s="1"/>
+    </row>
+    <row r="170" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1"/>
+      <c r="I170" s="1"/>
+      <c r="J170" s="1"/>
+      <c r="K170" s="1"/>
+      <c r="L170" s="1"/>
+      <c r="M170" s="1"/>
+      <c r="N170" s="1"/>
+      <c r="O170" s="1"/>
+      <c r="P170" s="1"/>
+      <c r="Q170" s="1"/>
+      <c r="R170" s="1"/>
+      <c r="S170" s="1"/>
+      <c r="T170" s="1"/>
+    </row>
+    <row r="171" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1"/>
+      <c r="I171" s="1"/>
+      <c r="J171" s="1"/>
+      <c r="K171" s="1"/>
+      <c r="L171" s="1"/>
+      <c r="M171" s="1"/>
+      <c r="N171" s="1"/>
+      <c r="O171" s="1"/>
+      <c r="P171" s="1"/>
+      <c r="Q171" s="1"/>
+      <c r="R171" s="1"/>
+      <c r="S171" s="1"/>
+      <c r="T171" s="1"/>
+    </row>
+    <row r="172" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1"/>
+      <c r="I172" s="1"/>
+      <c r="J172" s="1"/>
+      <c r="K172" s="1"/>
+      <c r="L172" s="1"/>
+      <c r="M172" s="1"/>
+      <c r="N172" s="1"/>
+      <c r="O172" s="1"/>
+      <c r="P172" s="1"/>
+      <c r="Q172" s="1"/>
+      <c r="R172" s="1"/>
+      <c r="S172" s="1"/>
+      <c r="T172" s="1"/>
+    </row>
+    <row r="173" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="1"/>
+      <c r="H173" s="1"/>
+      <c r="I173" s="1"/>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+      <c r="L173" s="1"/>
+      <c r="M173" s="1"/>
+      <c r="N173" s="1"/>
+      <c r="O173" s="1"/>
+      <c r="P173" s="1"/>
+      <c r="Q173" s="1"/>
+      <c r="R173" s="1"/>
+      <c r="S173" s="1"/>
+      <c r="T173" s="1"/>
+    </row>
+    <row r="174" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
+      <c r="H174" s="1"/>
+      <c r="I174" s="1"/>
+      <c r="J174" s="1"/>
+      <c r="K174" s="1"/>
+      <c r="L174" s="1"/>
+      <c r="M174" s="1"/>
+      <c r="N174" s="1"/>
+      <c r="O174" s="1"/>
+      <c r="P174" s="1"/>
+      <c r="Q174" s="1"/>
+      <c r="R174" s="1"/>
+      <c r="S174" s="1"/>
+      <c r="T174" s="1"/>
+    </row>
+    <row r="175" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1"/>
+      <c r="H175" s="1"/>
+      <c r="I175" s="1"/>
+      <c r="J175" s="1"/>
+      <c r="K175" s="1"/>
+      <c r="L175" s="1"/>
+      <c r="M175" s="1"/>
+      <c r="N175" s="1"/>
+      <c r="O175" s="1"/>
+      <c r="P175" s="1"/>
+      <c r="Q175" s="1"/>
+      <c r="R175" s="1"/>
+      <c r="S175" s="1"/>
+      <c r="T175" s="1"/>
+    </row>
+    <row r="176" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+      <c r="G176" s="1"/>
+      <c r="H176" s="1"/>
+      <c r="I176" s="1"/>
+      <c r="J176" s="1"/>
+      <c r="K176" s="1"/>
+      <c r="L176" s="1"/>
+      <c r="M176" s="1"/>
+      <c r="N176" s="1"/>
+      <c r="O176" s="1"/>
+      <c r="P176" s="1"/>
+      <c r="Q176" s="1"/>
+      <c r="R176" s="1"/>
+      <c r="S176" s="1"/>
+      <c r="T176" s="1"/>
+    </row>
+    <row r="177" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="1"/>
+      <c r="G177" s="1"/>
+      <c r="H177" s="1"/>
+      <c r="I177" s="1"/>
+      <c r="J177" s="1"/>
+      <c r="K177" s="1"/>
+      <c r="L177" s="1"/>
+      <c r="M177" s="1"/>
+      <c r="N177" s="1"/>
+      <c r="O177" s="1"/>
+      <c r="P177" s="1"/>
+      <c r="Q177" s="1"/>
+      <c r="R177" s="1"/>
+      <c r="S177" s="1"/>
+      <c r="T177" s="1"/>
+    </row>
+    <row r="178" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="1"/>
+      <c r="H178" s="1"/>
+      <c r="I178" s="1"/>
+      <c r="J178" s="1"/>
+      <c r="K178" s="1"/>
+      <c r="L178" s="1"/>
+      <c r="M178" s="1"/>
+      <c r="N178" s="1"/>
+      <c r="O178" s="1"/>
+      <c r="P178" s="1"/>
+      <c r="Q178" s="1"/>
+      <c r="R178" s="1"/>
+      <c r="S178" s="1"/>
+      <c r="T178" s="1"/>
+    </row>
+    <row r="179" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+      <c r="G179" s="1"/>
+      <c r="H179" s="1"/>
+      <c r="I179" s="1"/>
+      <c r="J179" s="1"/>
+      <c r="K179" s="1"/>
+      <c r="L179" s="1"/>
+      <c r="M179" s="1"/>
+      <c r="N179" s="1"/>
+      <c r="O179" s="1"/>
+      <c r="P179" s="1"/>
+      <c r="Q179" s="1"/>
+      <c r="R179" s="1"/>
+      <c r="S179" s="1"/>
+      <c r="T179" s="1"/>
+    </row>
+    <row r="180" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+      <c r="G180" s="1"/>
+      <c r="H180" s="1"/>
+      <c r="I180" s="1"/>
+      <c r="J180" s="1"/>
+      <c r="K180" s="1"/>
+      <c r="L180" s="1"/>
+      <c r="M180" s="1"/>
+      <c r="N180" s="1"/>
+      <c r="O180" s="1"/>
+      <c r="P180" s="1"/>
+      <c r="Q180" s="1"/>
+      <c r="R180" s="1"/>
+      <c r="S180" s="1"/>
+      <c r="T180" s="1"/>
+    </row>
+    <row r="181" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="1"/>
+      <c r="H181" s="1"/>
+      <c r="I181" s="1"/>
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+      <c r="L181" s="1"/>
+      <c r="M181" s="1"/>
+      <c r="N181" s="1"/>
+      <c r="O181" s="1"/>
+      <c r="P181" s="1"/>
+      <c r="Q181" s="1"/>
+      <c r="R181" s="1"/>
+      <c r="S181" s="1"/>
+      <c r="T181" s="1"/>
+    </row>
+    <row r="182" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C182" s="1"/>
+      <c r="D182" s="1"/>
+      <c r="E182" s="1"/>
+      <c r="F182" s="1"/>
+      <c r="G182" s="1"/>
+      <c r="H182" s="1"/>
+      <c r="I182" s="1"/>
+      <c r="J182" s="1"/>
+      <c r="K182" s="1"/>
+      <c r="L182" s="1"/>
+      <c r="M182" s="1"/>
+      <c r="N182" s="1"/>
+      <c r="O182" s="1"/>
+      <c r="P182" s="1"/>
+      <c r="Q182" s="1"/>
+      <c r="R182" s="1"/>
+      <c r="S182" s="1"/>
+      <c r="T182" s="1"/>
+    </row>
+    <row r="183" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C183" s="1"/>
+      <c r="D183" s="1"/>
+      <c r="E183" s="1"/>
+      <c r="F183" s="1"/>
+      <c r="G183" s="1"/>
+      <c r="H183" s="1"/>
+      <c r="I183" s="1"/>
+      <c r="J183" s="1"/>
+      <c r="K183" s="1"/>
+      <c r="L183" s="1"/>
+      <c r="M183" s="1"/>
+      <c r="N183" s="1"/>
+      <c r="O183" s="1"/>
+      <c r="P183" s="1"/>
+      <c r="Q183" s="1"/>
+      <c r="R183" s="1"/>
+      <c r="S183" s="1"/>
+      <c r="T183" s="1"/>
+    </row>
+    <row r="184" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C184" s="1"/>
+      <c r="D184" s="1"/>
+      <c r="E184" s="1"/>
+      <c r="F184" s="1"/>
+      <c r="G184" s="1"/>
+      <c r="H184" s="1"/>
+      <c r="I184" s="1"/>
+      <c r="J184" s="1"/>
+      <c r="K184" s="1"/>
+      <c r="L184" s="1"/>
+      <c r="M184" s="1"/>
+      <c r="N184" s="1"/>
+      <c r="O184" s="1"/>
+      <c r="P184" s="1"/>
+      <c r="Q184" s="1"/>
+      <c r="R184" s="1"/>
+      <c r="S184" s="1"/>
+      <c r="T184" s="1"/>
+    </row>
+    <row r="185" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C185" s="1"/>
+      <c r="D185" s="1"/>
+      <c r="E185" s="1"/>
+      <c r="F185" s="1"/>
+      <c r="G185" s="1"/>
+      <c r="H185" s="1"/>
+      <c r="I185" s="1"/>
+      <c r="J185" s="1"/>
+      <c r="K185" s="1"/>
+      <c r="L185" s="1"/>
+      <c r="M185" s="1"/>
+      <c r="N185" s="1"/>
+      <c r="O185" s="1"/>
+      <c r="P185" s="1"/>
+      <c r="Q185" s="1"/>
+      <c r="R185" s="1"/>
+      <c r="S185" s="1"/>
+      <c r="T185" s="1"/>
+    </row>
+    <row r="186" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
+      <c r="E186" s="1"/>
+      <c r="F186" s="1"/>
+      <c r="G186" s="1"/>
+      <c r="H186" s="1"/>
+      <c r="I186" s="1"/>
+      <c r="J186" s="1"/>
+      <c r="K186" s="1"/>
+      <c r="L186" s="1"/>
+      <c r="M186" s="1"/>
+      <c r="N186" s="1"/>
+      <c r="O186" s="1"/>
+      <c r="P186" s="1"/>
+      <c r="Q186" s="1"/>
+      <c r="R186" s="1"/>
+      <c r="S186" s="1"/>
+      <c r="T186" s="1"/>
+    </row>
+    <row r="187" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C187" s="1"/>
+      <c r="D187" s="1"/>
+      <c r="E187" s="1"/>
+      <c r="F187" s="1"/>
+      <c r="G187" s="1"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+      <c r="L187" s="1"/>
+      <c r="M187" s="1"/>
+      <c r="N187" s="1"/>
+      <c r="O187" s="1"/>
+      <c r="P187" s="1"/>
+      <c r="Q187" s="1"/>
+      <c r="R187" s="1"/>
+      <c r="S187" s="1"/>
+      <c r="T187" s="1"/>
+    </row>
+    <row r="188" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C188" s="1"/>
+      <c r="D188" s="1"/>
+      <c r="E188" s="1"/>
+      <c r="F188" s="1"/>
+      <c r="G188" s="1"/>
+      <c r="H188" s="1"/>
+      <c r="I188" s="1"/>
+      <c r="J188" s="1"/>
+      <c r="K188" s="1"/>
+      <c r="L188" s="1"/>
+      <c r="M188" s="1"/>
+      <c r="N188" s="1"/>
+      <c r="O188" s="1"/>
+      <c r="P188" s="1"/>
+      <c r="Q188" s="1"/>
+      <c r="R188" s="1"/>
+      <c r="S188" s="1"/>
+      <c r="T188" s="1"/>
+    </row>
+    <row r="189" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C189" s="1"/>
+      <c r="D189" s="1"/>
+      <c r="E189" s="1"/>
+      <c r="F189" s="1"/>
+      <c r="G189" s="1"/>
+      <c r="H189" s="1"/>
+      <c r="I189" s="1"/>
+      <c r="J189" s="1"/>
+      <c r="K189" s="1"/>
+      <c r="L189" s="1"/>
+      <c r="M189" s="1"/>
+      <c r="N189" s="1"/>
+      <c r="O189" s="1"/>
+      <c r="P189" s="1"/>
+      <c r="Q189" s="1"/>
+      <c r="R189" s="1"/>
+      <c r="S189" s="1"/>
+      <c r="T189" s="1"/>
+    </row>
+    <row r="190" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C190" s="1"/>
+      <c r="D190" s="1"/>
+      <c r="E190" s="1"/>
+      <c r="F190" s="1"/>
+      <c r="G190" s="1"/>
+      <c r="H190" s="1"/>
+      <c r="I190" s="1"/>
+      <c r="J190" s="1"/>
+      <c r="K190" s="1"/>
+      <c r="L190" s="1"/>
+      <c r="M190" s="1"/>
+      <c r="N190" s="1"/>
+      <c r="O190" s="1"/>
+      <c r="P190" s="1"/>
+      <c r="Q190" s="1"/>
+      <c r="R190" s="1"/>
+      <c r="S190" s="1"/>
+      <c r="T190" s="1"/>
+    </row>
+    <row r="191" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C191" s="1"/>
+      <c r="D191" s="1"/>
+      <c r="E191" s="1"/>
+      <c r="F191" s="1"/>
+      <c r="G191" s="1"/>
+      <c r="H191" s="1"/>
+      <c r="I191" s="1"/>
+      <c r="J191" s="1"/>
+      <c r="K191" s="1"/>
+      <c r="L191" s="1"/>
+      <c r="M191" s="1"/>
+      <c r="N191" s="1"/>
+      <c r="O191" s="1"/>
+      <c r="P191" s="1"/>
+      <c r="Q191" s="1"/>
+      <c r="R191" s="1"/>
+      <c r="S191" s="1"/>
+      <c r="T191" s="1"/>
+    </row>
+    <row r="192" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C192" s="1"/>
+      <c r="D192" s="1"/>
+      <c r="E192" s="1"/>
+      <c r="F192" s="1"/>
+      <c r="G192" s="1"/>
+      <c r="H192" s="1"/>
+      <c r="I192" s="1"/>
+      <c r="J192" s="1"/>
+      <c r="K192" s="1"/>
+      <c r="L192" s="1"/>
+      <c r="M192" s="1"/>
+      <c r="N192" s="1"/>
+      <c r="O192" s="1"/>
+      <c r="P192" s="1"/>
+      <c r="Q192" s="1"/>
+      <c r="R192" s="1"/>
+      <c r="S192" s="1"/>
+      <c r="T192" s="1"/>
+    </row>
+    <row r="193" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C193" s="1"/>
+      <c r="D193" s="1"/>
+      <c r="E193" s="1"/>
+      <c r="F193" s="1"/>
+      <c r="G193" s="1"/>
+      <c r="H193" s="1"/>
+      <c r="I193" s="1"/>
+      <c r="J193" s="1"/>
+      <c r="K193" s="1"/>
+      <c r="L193" s="1"/>
+      <c r="M193" s="1"/>
+      <c r="N193" s="1"/>
+      <c r="O193" s="1"/>
+      <c r="P193" s="1"/>
+      <c r="Q193" s="1"/>
+      <c r="R193" s="1"/>
+      <c r="S193" s="1"/>
+      <c r="T193" s="1"/>
+    </row>
+    <row r="194" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C194" s="1"/>
+      <c r="D194" s="1"/>
+      <c r="E194" s="1"/>
+      <c r="F194" s="1"/>
+      <c r="G194" s="1"/>
+      <c r="H194" s="1"/>
+      <c r="I194" s="1"/>
+      <c r="J194" s="1"/>
+      <c r="K194" s="1"/>
+      <c r="L194" s="1"/>
+      <c r="M194" s="1"/>
+      <c r="N194" s="1"/>
+      <c r="O194" s="1"/>
+      <c r="P194" s="1"/>
+      <c r="Q194" s="1"/>
+      <c r="R194" s="1"/>
+      <c r="S194" s="1"/>
+      <c r="T194" s="1"/>
+    </row>
+    <row r="195" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C195" s="1"/>
+      <c r="D195" s="1"/>
+      <c r="E195" s="1"/>
+      <c r="F195" s="1"/>
+      <c r="G195" s="1"/>
+      <c r="H195" s="1"/>
+      <c r="I195" s="1"/>
+      <c r="J195" s="1"/>
+      <c r="K195" s="1"/>
+      <c r="L195" s="1"/>
+      <c r="M195" s="1"/>
+      <c r="N195" s="1"/>
+      <c r="O195" s="1"/>
+      <c r="P195" s="1"/>
+      <c r="Q195" s="1"/>
+      <c r="R195" s="1"/>
+      <c r="S195" s="1"/>
+      <c r="T195" s="1"/>
+    </row>
+    <row r="196" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C196" s="1"/>
+      <c r="D196" s="1"/>
+      <c r="E196" s="1"/>
+      <c r="F196" s="1"/>
+      <c r="G196" s="1"/>
+      <c r="H196" s="1"/>
+      <c r="I196" s="1"/>
+      <c r="J196" s="1"/>
+      <c r="K196" s="1"/>
+      <c r="L196" s="1"/>
+      <c r="M196" s="1"/>
+      <c r="N196" s="1"/>
+      <c r="O196" s="1"/>
+      <c r="P196" s="1"/>
+      <c r="Q196" s="1"/>
+      <c r="R196" s="1"/>
+      <c r="S196" s="1"/>
+      <c r="T196" s="1"/>
+    </row>
+    <row r="197" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C197" s="1"/>
+      <c r="D197" s="1"/>
+      <c r="E197" s="1"/>
+      <c r="F197" s="1"/>
+      <c r="G197" s="1"/>
+      <c r="H197" s="1"/>
+      <c r="I197" s="1"/>
+      <c r="J197" s="1"/>
+      <c r="K197" s="1"/>
+      <c r="L197" s="1"/>
+      <c r="M197" s="1"/>
+      <c r="N197" s="1"/>
+      <c r="O197" s="1"/>
+      <c r="P197" s="1"/>
+      <c r="Q197" s="1"/>
+      <c r="R197" s="1"/>
+      <c r="S197" s="1"/>
+      <c r="T197" s="1"/>
+    </row>
+    <row r="198" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C198" s="1"/>
+      <c r="D198" s="1"/>
+      <c r="E198" s="1"/>
+      <c r="F198" s="1"/>
+      <c r="G198" s="1"/>
+      <c r="H198" s="1"/>
+      <c r="I198" s="1"/>
+      <c r="J198" s="1"/>
+      <c r="K198" s="1"/>
+      <c r="L198" s="1"/>
+      <c r="M198" s="1"/>
+      <c r="N198" s="1"/>
+      <c r="O198" s="1"/>
+      <c r="P198" s="1"/>
+      <c r="Q198" s="1"/>
+      <c r="R198" s="1"/>
+      <c r="S198" s="1"/>
+      <c r="T198" s="1"/>
+    </row>
+    <row r="199" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C199" s="1"/>
+      <c r="D199" s="1"/>
+      <c r="E199" s="1"/>
+      <c r="F199" s="1"/>
+      <c r="G199" s="1"/>
+      <c r="H199" s="1"/>
+      <c r="I199" s="1"/>
+      <c r="J199" s="1"/>
+      <c r="K199" s="1"/>
+      <c r="L199" s="1"/>
+      <c r="M199" s="1"/>
+      <c r="N199" s="1"/>
+      <c r="O199" s="1"/>
+      <c r="P199" s="1"/>
+      <c r="Q199" s="1"/>
+      <c r="R199" s="1"/>
+      <c r="S199" s="1"/>
+      <c r="T199" s="1"/>
+    </row>
+    <row r="200" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C200" s="1"/>
+      <c r="D200" s="1"/>
+      <c r="E200" s="1"/>
+      <c r="F200" s="1"/>
+      <c r="G200" s="1"/>
+      <c r="H200" s="1"/>
+      <c r="I200" s="1"/>
+      <c r="J200" s="1"/>
+      <c r="K200" s="1"/>
+      <c r="L200" s="1"/>
+      <c r="M200" s="1"/>
+      <c r="N200" s="1"/>
+      <c r="O200" s="1"/>
+      <c r="P200" s="1"/>
+      <c r="Q200" s="1"/>
+      <c r="R200" s="1"/>
+      <c r="S200" s="1"/>
+      <c r="T200" s="1"/>
+    </row>
+    <row r="201" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C201" s="1"/>
+      <c r="D201" s="1"/>
+      <c r="E201" s="1"/>
+      <c r="F201" s="1"/>
+      <c r="G201" s="1"/>
+      <c r="H201" s="1"/>
+      <c r="I201" s="1"/>
+      <c r="J201" s="1"/>
+      <c r="K201" s="1"/>
+      <c r="L201" s="1"/>
+      <c r="M201" s="1"/>
+      <c r="N201" s="1"/>
+      <c r="O201" s="1"/>
+      <c r="P201" s="1"/>
+      <c r="Q201" s="1"/>
+      <c r="R201" s="1"/>
+      <c r="S201" s="1"/>
+      <c r="T201" s="1"/>
+    </row>
+    <row r="202" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C202" s="1"/>
+      <c r="D202" s="1"/>
+      <c r="E202" s="1"/>
+      <c r="F202" s="1"/>
+      <c r="G202" s="1"/>
+      <c r="H202" s="1"/>
+      <c r="I202" s="1"/>
+      <c r="J202" s="1"/>
+      <c r="K202" s="1"/>
+      <c r="L202" s="1"/>
+      <c r="M202" s="1"/>
+      <c r="N202" s="1"/>
+      <c r="O202" s="1"/>
+      <c r="P202" s="1"/>
+      <c r="Q202" s="1"/>
+      <c r="R202" s="1"/>
+      <c r="S202" s="1"/>
+      <c r="T202" s="1"/>
+    </row>
+    <row r="203" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C203" s="1"/>
+      <c r="D203" s="1"/>
+      <c r="E203" s="1"/>
+      <c r="F203" s="1"/>
+      <c r="G203" s="1"/>
+      <c r="H203" s="1"/>
+      <c r="I203" s="1"/>
+      <c r="J203" s="1"/>
+      <c r="K203" s="1"/>
+      <c r="L203" s="1"/>
+      <c r="M203" s="1"/>
+      <c r="N203" s="1"/>
+      <c r="O203" s="1"/>
+      <c r="P203" s="1"/>
+      <c r="Q203" s="1"/>
+      <c r="R203" s="1"/>
+      <c r="S203" s="1"/>
+      <c r="T203" s="1"/>
+    </row>
+    <row r="204" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+      <c r="E204" s="1"/>
+      <c r="F204" s="1"/>
+      <c r="G204" s="1"/>
+      <c r="H204" s="1"/>
+      <c r="I204" s="1"/>
+      <c r="J204" s="1"/>
+      <c r="K204" s="1"/>
+      <c r="L204" s="1"/>
+      <c r="M204" s="1"/>
+      <c r="N204" s="1"/>
+      <c r="O204" s="1"/>
+      <c r="P204" s="1"/>
+      <c r="Q204" s="1"/>
+      <c r="R204" s="1"/>
+      <c r="S204" s="1"/>
+      <c r="T204" s="1"/>
+    </row>
+    <row r="205" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C205" s="1"/>
+      <c r="D205" s="1"/>
+      <c r="E205" s="1"/>
+      <c r="F205" s="1"/>
+      <c r="G205" s="1"/>
+      <c r="H205" s="1"/>
+      <c r="I205" s="1"/>
+      <c r="J205" s="1"/>
+      <c r="K205" s="1"/>
+      <c r="L205" s="1"/>
+      <c r="M205" s="1"/>
+      <c r="N205" s="1"/>
+      <c r="O205" s="1"/>
+      <c r="P205" s="1"/>
+      <c r="Q205" s="1"/>
+      <c r="R205" s="1"/>
+      <c r="S205" s="1"/>
+      <c r="T205" s="1"/>
+    </row>
+    <row r="206" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C206" s="1"/>
+      <c r="D206" s="1"/>
+      <c r="E206" s="1"/>
+      <c r="F206" s="1"/>
+      <c r="G206" s="1"/>
+      <c r="H206" s="1"/>
+      <c r="I206" s="1"/>
+      <c r="J206" s="1"/>
+      <c r="K206" s="1"/>
+      <c r="L206" s="1"/>
+      <c r="M206" s="1"/>
+      <c r="N206" s="1"/>
+      <c r="O206" s="1"/>
+      <c r="P206" s="1"/>
+      <c r="Q206" s="1"/>
+      <c r="R206" s="1"/>
+      <c r="S206" s="1"/>
+      <c r="T206" s="1"/>
+    </row>
+    <row r="207" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C207" s="1"/>
+      <c r="D207" s="1"/>
+      <c r="E207" s="1"/>
+      <c r="F207" s="1"/>
+      <c r="G207" s="1"/>
+      <c r="H207" s="1"/>
+      <c r="I207" s="1"/>
+      <c r="J207" s="1"/>
+      <c r="K207" s="1"/>
+      <c r="L207" s="1"/>
+      <c r="M207" s="1"/>
+      <c r="N207" s="1"/>
+      <c r="O207" s="1"/>
+      <c r="P207" s="1"/>
+      <c r="Q207" s="1"/>
+      <c r="R207" s="1"/>
+      <c r="S207" s="1"/>
+      <c r="T207" s="1"/>
+    </row>
+    <row r="208" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C208" s="1"/>
+      <c r="D208" s="1"/>
+      <c r="E208" s="1"/>
+      <c r="F208" s="1"/>
+      <c r="G208" s="1"/>
+      <c r="H208" s="1"/>
+      <c r="I208" s="1"/>
+      <c r="J208" s="1"/>
+      <c r="K208" s="1"/>
+      <c r="L208" s="1"/>
+      <c r="M208" s="1"/>
+      <c r="N208" s="1"/>
+      <c r="O208" s="1"/>
+      <c r="P208" s="1"/>
+      <c r="Q208" s="1"/>
+      <c r="R208" s="1"/>
+      <c r="S208" s="1"/>
+      <c r="T208" s="1"/>
+    </row>
+    <row r="209" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C209" s="1"/>
+      <c r="D209" s="1"/>
+      <c r="E209" s="1"/>
+      <c r="F209" s="1"/>
+      <c r="G209" s="1"/>
+      <c r="H209" s="1"/>
+      <c r="I209" s="1"/>
+      <c r="J209" s="1"/>
+      <c r="K209" s="1"/>
+      <c r="L209" s="1"/>
+      <c r="M209" s="1"/>
+      <c r="N209" s="1"/>
+      <c r="O209" s="1"/>
+      <c r="P209" s="1"/>
+      <c r="Q209" s="1"/>
+      <c r="R209" s="1"/>
+      <c r="S209" s="1"/>
+      <c r="T209" s="1"/>
+    </row>
+    <row r="210" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C210" s="1"/>
+      <c r="D210" s="1"/>
+      <c r="E210" s="1"/>
+      <c r="F210" s="1"/>
+      <c r="G210" s="1"/>
+      <c r="H210" s="1"/>
+      <c r="I210" s="1"/>
+      <c r="J210" s="1"/>
+      <c r="K210" s="1"/>
+      <c r="L210" s="1"/>
+      <c r="M210" s="1"/>
+      <c r="N210" s="1"/>
+      <c r="O210" s="1"/>
+      <c r="P210" s="1"/>
+      <c r="Q210" s="1"/>
+      <c r="R210" s="1"/>
+      <c r="S210" s="1"/>
+      <c r="T210" s="1"/>
+    </row>
+    <row r="212" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C212" s="1"/>
+      <c r="D212" s="1"/>
+      <c r="E212" s="1"/>
+      <c r="F212" s="1"/>
+      <c r="G212" s="1"/>
+      <c r="H212" s="1"/>
+      <c r="I212" s="1"/>
+      <c r="J212" s="1"/>
+      <c r="K212" s="1"/>
+      <c r="L212" s="1"/>
+      <c r="M212" s="1"/>
+      <c r="N212" s="1"/>
+      <c r="O212" s="1"/>
+      <c r="P212" s="1"/>
+      <c r="Q212" s="1"/>
+      <c r="R212" s="1"/>
+      <c r="S212" s="1"/>
+      <c r="T212" s="1"/>
+    </row>
+    <row r="218" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="G218" s="1"/>
+    </row>
+    <row r="221" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C221" s="1"/>
+      <c r="D221" s="1"/>
+      <c r="E221" s="1"/>
+      <c r="F221" s="1"/>
+      <c r="G221" s="1"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>